<commit_message>
changed the data file and added visualization file
</commit_message>
<xml_diff>
--- a/SCMS_Delivery_History_Dataset(FOR USE).xlsx
+++ b/SCMS_Delivery_History_Dataset(FOR USE).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01-SDE\8-Unipd2023\2023-DataBase2\Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01-SDE\8-Unipd2023\2023-DataBase2\Code\20231206\DB2-RDF-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6B0B3B-AB0C-46C0-892A-D35A1EF528B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB27B6C-BB27-4593-B8C4-A779F461ED69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -715,56 +715,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1048,1430 +1039,1433 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z8" sqref="Z8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" style="7"/>
+    <col min="1" max="1" width="9.06640625" style="5"/>
     <col min="3" max="3" width="17.3984375" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="34" customWidth="1"/>
-    <col min="7" max="7" width="35.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.3984375" customWidth="1"/>
     <col min="8" max="8" width="15.1328125" customWidth="1"/>
     <col min="10" max="10" width="18.1328125" customWidth="1"/>
     <col min="11" max="11" width="17.796875" customWidth="1"/>
     <col min="12" max="12" width="16.3984375" customWidth="1"/>
     <col min="13" max="13" width="19.46484375" customWidth="1"/>
     <col min="14" max="14" width="18.6640625" customWidth="1"/>
-    <col min="23" max="23" width="32.6640625" style="17" customWidth="1"/>
-    <col min="27" max="27" width="9.06640625" style="17"/>
+    <col min="23" max="23" width="32.6640625" style="3" customWidth="1"/>
+    <col min="27" max="27" width="9.06640625" style="3"/>
     <col min="28" max="28" width="20.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="4" customFormat="1" ht="41.65">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:33" s="2" customFormat="1" ht="41.65">
+      <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="R1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AC1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AD1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AE1" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AG1" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="1" customFormat="1" ht="55.5">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:33" s="1" customFormat="1">
+      <c r="A2" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="10">
         <v>719</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="11">
         <v>39880</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="12">
         <v>39836</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="12">
         <v>39836</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="12">
         <v>39836</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="R2" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="S2" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="T2" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="U2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="V2" s="1">
+      <c r="V2" s="10">
         <v>12830.91</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="W2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="X2" s="1">
+      <c r="X2" s="10">
         <v>19.11</v>
       </c>
-      <c r="Y2" s="1">
+      <c r="Y2" s="10">
         <v>25000</v>
       </c>
-      <c r="Z2" s="1">
+      <c r="Z2" s="10">
         <v>9750</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AA2" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AB2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="AC2" s="1">
+      <c r="AC2" s="10">
         <v>0.39</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AD2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="AE2" s="1">
+      <c r="AE2" s="10">
         <v>0.03</v>
       </c>
-      <c r="AF2" s="1">
+      <c r="AF2" s="10">
         <v>12</v>
       </c>
-      <c r="AG2" s="1">
+      <c r="AG2" s="10">
         <v>1708</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="1" customFormat="1" ht="69.400000000000006">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:33" s="1" customFormat="1">
+      <c r="A3" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="10">
         <v>630</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="11">
         <v>39121</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K3" s="12">
         <v>39700</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="12">
         <v>39700</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="N3" s="3">
+      <c r="N3" s="12">
         <v>39869</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="R3" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="S3" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="T3" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="U3" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="V3" s="1">
+      <c r="V3" s="10">
         <v>1755.87</v>
       </c>
-      <c r="W3" s="4" t="s">
+      <c r="W3" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="X3" s="1">
+      <c r="X3" s="10">
         <v>2.48</v>
       </c>
-      <c r="Y3" s="1">
+      <c r="Y3" s="10">
         <v>34</v>
       </c>
-      <c r="Z3" s="1">
+      <c r="Z3" s="10">
         <v>1547.68</v>
       </c>
-      <c r="AA3" s="4" t="s">
+      <c r="AA3" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AB3" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="AC3" s="1">
+      <c r="AC3" s="10">
         <v>45.52</v>
       </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AD3" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="AE3" s="1">
+      <c r="AE3" s="10">
         <v>0.08</v>
       </c>
-      <c r="AF3" s="1">
+      <c r="AF3" s="10">
         <v>540</v>
       </c>
-      <c r="AG3" s="1">
+      <c r="AG3" s="10">
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:33" s="11" customFormat="1" ht="55.5">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:33" s="4" customFormat="1">
+      <c r="A4" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="9">
         <v>41238</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="13">
         <v>37514</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="14">
         <v>42197</v>
       </c>
-      <c r="L4" s="10">
+      <c r="L4" s="14">
         <v>42198</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="M4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="N4" s="10">
+      <c r="N4" s="14">
         <v>42197</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="O4" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="P4" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="Q4" s="8" t="s">
+      <c r="Q4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="R4" s="8" t="s">
+      <c r="R4" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="S4" s="8" t="s">
+      <c r="S4" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="T4" s="8" t="s">
+      <c r="T4" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="U4" s="8" t="s">
+      <c r="U4" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="V4" s="8">
+      <c r="V4" s="9">
         <v>555.49</v>
       </c>
-      <c r="W4" s="8" t="s">
+      <c r="W4" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="X4" s="8">
+      <c r="X4" s="9">
         <v>0.94</v>
       </c>
-      <c r="Y4" s="8">
+      <c r="Y4" s="9">
         <v>32</v>
       </c>
-      <c r="Z4" s="8">
+      <c r="Z4" s="9">
         <v>800</v>
       </c>
-      <c r="AA4" s="8" t="s">
+      <c r="AA4" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="AB4" s="8" t="s">
+      <c r="AB4" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="AC4" s="8">
+      <c r="AC4" s="9">
         <v>25</v>
       </c>
-      <c r="AD4" s="8" t="s">
+      <c r="AD4" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="AE4" s="8">
+      <c r="AE4" s="9">
         <v>0.25</v>
       </c>
-      <c r="AF4" s="8">
+      <c r="AF4" s="9">
         <v>100</v>
       </c>
-      <c r="AG4" s="8">
+      <c r="AG4" s="9">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:33" s="8" customFormat="1" ht="55.5">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:33" s="2" customFormat="1">
+      <c r="A5" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="10">
         <v>40351</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="11">
         <v>41101</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="K5" s="16">
+      <c r="K5" s="12">
         <v>40926</v>
       </c>
-      <c r="L5" s="16">
+      <c r="L5" s="12">
         <v>40926</v>
       </c>
-      <c r="M5" s="14" t="s">
+      <c r="M5" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="N5" s="16">
+      <c r="N5" s="12">
         <v>40926</v>
       </c>
-      <c r="O5" s="14" t="s">
+      <c r="O5" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="P5" s="14" t="s">
+      <c r="P5" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="Q5" s="14" t="s">
+      <c r="Q5" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="R5" s="14" t="s">
+      <c r="R5" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="S5" s="14" t="s">
+      <c r="S5" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="T5" s="14" t="s">
+      <c r="T5" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="U5" s="14" t="s">
+      <c r="U5" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="V5" s="14" t="s">
+      <c r="V5" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="W5" s="8" t="s">
+      <c r="W5" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="X5" s="14">
+      <c r="X5" s="10">
         <v>0.44</v>
       </c>
-      <c r="Y5" s="14">
+      <c r="Y5" s="10">
         <v>10</v>
       </c>
-      <c r="Z5" s="14">
+      <c r="Z5" s="10">
         <v>316.5</v>
       </c>
-      <c r="AA5" s="8" t="s">
+      <c r="AA5" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="AB5" s="14" t="s">
+      <c r="AB5" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="AC5" s="14">
+      <c r="AC5" s="10">
         <v>31.65</v>
       </c>
-      <c r="AD5" s="14" t="s">
+      <c r="AD5" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="AE5" s="14">
+      <c r="AE5" s="10">
         <v>0.03</v>
       </c>
-      <c r="AF5" s="14">
+      <c r="AF5" s="10">
         <v>1000</v>
       </c>
-      <c r="AG5" s="14" t="s">
+      <c r="AG5" s="10" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:33" s="1" customFormat="1" ht="55.5">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:33" s="1" customFormat="1">
+      <c r="A6" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="10">
         <v>15</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="12">
         <v>38961</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="12">
         <v>38961</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="12">
         <v>38961</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="O6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P6" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="R6" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="S6" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="T6" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="U6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="V6" s="1">
+      <c r="V6" s="10">
         <v>16007.06</v>
       </c>
-      <c r="W6" s="4" t="s">
+      <c r="W6" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="Y6" s="1">
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10">
         <v>31920</v>
       </c>
-      <c r="Z6" s="1">
+      <c r="Z6" s="10">
         <v>127360.8</v>
       </c>
-      <c r="AA6" s="4" t="s">
+      <c r="AA6" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AB6" s="1" t="s">
+      <c r="AB6" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="AC6" s="1">
+      <c r="AC6" s="10">
         <v>3.99</v>
       </c>
-      <c r="AD6" s="1" t="s">
+      <c r="AD6" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="AE6" s="1">
+      <c r="AE6" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AF6" s="1">
+      <c r="AF6" s="10">
         <v>60</v>
       </c>
-      <c r="AG6" s="1">
+      <c r="AG6" s="10">
         <v>1855</v>
       </c>
     </row>
-    <row r="7" spans="1:33" s="1" customFormat="1" ht="41.65">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:33" s="1" customFormat="1">
+      <c r="A7" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="10">
         <v>16</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="12">
         <v>38940</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="12">
         <v>38940</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="12">
         <v>38940</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="R7" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="S7" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="T7" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="U7" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="V7" s="1">
+      <c r="V7" s="10">
         <v>45450.080000000002</v>
       </c>
-      <c r="W7" s="4" t="s">
+      <c r="W7" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="Y7" s="1">
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10">
         <v>38000</v>
       </c>
-      <c r="Z7" s="1">
+      <c r="Z7" s="10">
         <v>121600</v>
       </c>
-      <c r="AA7" s="4" t="s">
+      <c r="AA7" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="AB7" s="1" t="s">
+      <c r="AB7" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="AC7" s="1">
+      <c r="AC7" s="10">
         <v>3.2</v>
       </c>
-      <c r="AD7" s="1" t="s">
+      <c r="AD7" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="AE7" s="1">
+      <c r="AE7" s="10">
         <v>0.05</v>
       </c>
-      <c r="AF7" s="1">
+      <c r="AF7" s="10">
         <v>60</v>
       </c>
-      <c r="AG7" s="1">
+      <c r="AG7" s="10">
         <v>7590</v>
       </c>
     </row>
-    <row r="8" spans="1:33" s="1" customFormat="1" ht="41.65">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:33" s="1" customFormat="1">
+      <c r="A8" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="10">
         <v>11062</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="12">
         <v>40025</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8" s="12">
         <v>40025</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="M8" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="12">
         <v>40025</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O8" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="P8" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="R8" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="S8" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="T8" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="U8" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="V8" s="1">
+      <c r="V8" s="10">
         <v>6811.39</v>
       </c>
-      <c r="W8" s="4" t="s">
+      <c r="W8" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="X8" s="1">
+      <c r="X8" s="10">
         <v>4.79</v>
       </c>
-      <c r="Y8" s="1">
+      <c r="Y8" s="10">
         <v>1092</v>
       </c>
-      <c r="Z8" s="1">
+      <c r="Z8" s="10">
         <v>2446.08</v>
       </c>
-      <c r="AA8" s="4" t="s">
+      <c r="AA8" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="AB8" s="1" t="s">
+      <c r="AB8" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="AC8" s="1">
+      <c r="AC8" s="10">
         <v>2.2400000000000002</v>
       </c>
-      <c r="AD8" s="1" t="s">
+      <c r="AD8" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="AE8" s="1">
+      <c r="AE8" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AF8" s="1">
+      <c r="AF8" s="10">
         <v>30</v>
       </c>
-      <c r="AG8" s="1">
+      <c r="AG8" s="10">
         <v>1585</v>
       </c>
     </row>
-    <row r="9" spans="1:33" s="1" customFormat="1" ht="41.65">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:33" s="1" customFormat="1">
+      <c r="A9" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="10">
         <v>11063</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="12">
         <v>40025</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="12">
         <v>40025</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="M9" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="12">
         <v>40025</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="O9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="P9" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="Q9" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="R9" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="S9" s="1" t="s">
+      <c r="S9" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="T9" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="U9" s="1" t="s">
+      <c r="U9" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="V9" s="1" t="s">
+      <c r="V9" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="W9" s="4" t="s">
+      <c r="W9" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="X9" s="1">
+      <c r="X9" s="10">
         <v>8.67</v>
       </c>
-      <c r="Y9" s="1">
+      <c r="Y9" s="10">
         <v>2304</v>
       </c>
-      <c r="Z9" s="1">
+      <c r="Z9" s="10">
         <v>4423.68</v>
       </c>
-      <c r="AA9" s="4" t="s">
+      <c r="AA9" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="AB9" s="1" t="s">
+      <c r="AB9" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="AC9" s="1">
+      <c r="AC9" s="10">
         <v>1.92</v>
       </c>
-      <c r="AD9" s="1" t="s">
+      <c r="AD9" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="AE9" s="1">
+      <c r="AE9" s="10">
         <v>0.01</v>
       </c>
-      <c r="AF9" s="1">
+      <c r="AF9" s="10">
         <v>240</v>
       </c>
-      <c r="AG9" s="1" t="s">
+      <c r="AG9" s="10" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:33" s="1" customFormat="1" ht="55.5">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:33" s="1" customFormat="1">
+      <c r="A10" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="10">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10" s="12">
         <v>38870</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10" s="12">
         <v>38870</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="M10" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10" s="12">
         <v>38870</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="O10" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="P10" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="Q10" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="R10" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="S10" s="1" t="s">
+      <c r="S10" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="T10" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="U10" s="1" t="s">
+      <c r="U10" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="V10" s="1">
+      <c r="V10" s="10">
         <v>780.34</v>
       </c>
-      <c r="W10" s="4" t="s">
+      <c r="W10" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="Y10" s="1">
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10">
         <v>19</v>
       </c>
-      <c r="Z10" s="1">
+      <c r="Z10" s="10">
         <v>551</v>
       </c>
-      <c r="AA10" s="4" t="s">
+      <c r="AA10" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="AB10" s="1" t="s">
+      <c r="AB10" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="AC10" s="1">
+      <c r="AC10" s="10">
         <v>29</v>
       </c>
-      <c r="AD10" s="1" t="s">
+      <c r="AD10" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="AE10" s="1">
+      <c r="AE10" s="10">
         <v>0.97</v>
       </c>
-      <c r="AF10" s="1">
+      <c r="AF10" s="10">
         <v>30</v>
       </c>
-      <c r="AG10" s="1">
+      <c r="AG10" s="10">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:33" s="14" customFormat="1" ht="69.400000000000006">
-      <c r="A11" s="14" t="s">
+    <row r="11" spans="1:33" s="1" customFormat="1">
+      <c r="A11" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="10">
         <v>3378</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="I11" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="K11" s="16">
+      <c r="K11" s="12">
         <v>39861</v>
       </c>
-      <c r="L11" s="16">
+      <c r="L11" s="12">
         <v>39861</v>
       </c>
-      <c r="M11" s="14" t="s">
+      <c r="M11" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="N11" s="16">
+      <c r="N11" s="12">
         <v>39861</v>
       </c>
-      <c r="O11" s="14" t="s">
+      <c r="O11" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="P11" s="14" t="s">
+      <c r="P11" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="Q11" s="14" t="s">
+      <c r="Q11" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="R11" s="14" t="s">
+      <c r="R11" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="S11" s="14" t="s">
+      <c r="S11" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="T11" s="14" t="s">
+      <c r="T11" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="U11" s="14" t="s">
+      <c r="U11" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="V11" s="14">
+      <c r="V11" s="10">
         <v>3499.18</v>
       </c>
-      <c r="W11" s="8" t="s">
+      <c r="W11" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="X11" s="14">
+      <c r="X11" s="10">
         <v>156.80000000000001</v>
       </c>
-      <c r="Y11" s="14">
+      <c r="Y11" s="10">
         <v>1000</v>
       </c>
-      <c r="Z11" s="14">
+      <c r="Z11" s="10">
         <v>80000</v>
       </c>
-      <c r="AA11" s="8" t="s">
+      <c r="AA11" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="AB11" s="14" t="s">
+      <c r="AB11" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="AC11" s="14">
+      <c r="AC11" s="10">
         <v>80</v>
       </c>
-      <c r="AD11" s="14" t="s">
+      <c r="AD11" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="AE11" s="14">
+      <c r="AE11" s="10">
         <v>0.8</v>
       </c>
-      <c r="AF11" s="14">
+      <c r="AF11" s="10">
         <v>100</v>
       </c>
-      <c r="AG11" s="14">
+      <c r="AG11" s="10">
         <v>337</v>
       </c>
     </row>
-    <row r="12" spans="1:33" s="14" customFormat="1" ht="27.75">
-      <c r="A12" s="14" t="s">
+    <row r="12" spans="1:33" s="1" customFormat="1">
+      <c r="A12" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="10">
         <v>3386</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I12" s="14" t="s">
+      <c r="I12" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="J12" s="14" t="s">
+      <c r="J12" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="K12" s="16">
+      <c r="K12" s="12">
         <v>39724</v>
       </c>
-      <c r="L12" s="16">
+      <c r="L12" s="12">
         <v>39724</v>
       </c>
-      <c r="M12" s="14" t="s">
+      <c r="M12" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="N12" s="16">
+      <c r="N12" s="12">
         <v>39724</v>
       </c>
-      <c r="O12" s="14" t="s">
+      <c r="O12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="P12" s="14" t="s">
+      <c r="P12" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="Q12" s="14" t="s">
+      <c r="Q12" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="R12" s="14" t="s">
+      <c r="R12" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="S12" s="14" t="s">
+      <c r="S12" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="T12" s="14" t="s">
+      <c r="T12" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="U12" s="14" t="s">
+      <c r="U12" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="V12" s="14">
+      <c r="V12" s="10">
         <v>2648.82</v>
       </c>
-      <c r="W12" s="8" t="s">
+      <c r="W12" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="X12" s="14">
+      <c r="X12" s="10">
         <v>115.18</v>
       </c>
-      <c r="Y12" s="14">
+      <c r="Y12" s="10">
         <v>1000</v>
       </c>
-      <c r="Z12" s="14">
+      <c r="Z12" s="10">
         <v>71990</v>
       </c>
-      <c r="AA12" s="8" t="s">
+      <c r="AA12" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="AB12" s="14" t="s">
+      <c r="AB12" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="AC12" s="14">
+      <c r="AC12" s="10">
         <v>71.989999999999995</v>
       </c>
-      <c r="AD12" s="14" t="s">
+      <c r="AD12" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="AE12" s="14">
+      <c r="AE12" s="10">
         <v>0.72</v>
       </c>
-      <c r="AF12" s="14">
+      <c r="AF12" s="10">
         <v>100</v>
       </c>
-      <c r="AG12" s="14">
+      <c r="AG12" s="10">
         <v>296</v>
       </c>
     </row>
-    <row r="13" spans="1:33" s="11" customFormat="1" ht="41.65">
-      <c r="A13" s="11" t="s">
+    <row r="13" spans="1:33" s="4" customFormat="1">
+      <c r="A13" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="9">
         <v>1971</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="I13" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="J13" s="11" t="s">
+      <c r="J13" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K13" s="14">
         <v>39797</v>
       </c>
-      <c r="L13" s="12">
+      <c r="L13" s="14">
         <v>39797</v>
       </c>
-      <c r="M13" s="11" t="s">
+      <c r="M13" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="N13" s="12">
+      <c r="N13" s="14">
         <v>39797</v>
       </c>
-      <c r="O13" s="11" t="s">
+      <c r="O13" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="P13" s="11" t="s">
+      <c r="P13" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="Q13" s="11" t="s">
+      <c r="Q13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="R13" s="11" t="s">
+      <c r="R13" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="S13" s="11" t="s">
+      <c r="S13" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="T13" s="11" t="s">
+      <c r="T13" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="U13" s="11" t="s">
+      <c r="U13" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="V13" s="11">
+      <c r="V13" s="9">
         <v>648.27</v>
       </c>
-      <c r="W13" s="13" t="s">
+      <c r="W13" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="X13" s="11">
+      <c r="X13" s="9">
         <v>7.94</v>
       </c>
-      <c r="Y13" s="11">
+      <c r="Y13" s="9">
         <v>108</v>
       </c>
-      <c r="Z13" s="11">
+      <c r="Z13" s="9">
         <v>4050</v>
       </c>
-      <c r="AA13" s="13" t="s">
+      <c r="AA13" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="AB13" s="11" t="s">
+      <c r="AB13" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="AC13" s="11">
+      <c r="AC13" s="9">
         <v>37.5</v>
       </c>
-      <c r="AD13" s="11" t="s">
+      <c r="AD13" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="AE13" s="11">
+      <c r="AE13" s="9">
         <v>1.5</v>
       </c>
-      <c r="AF13" s="11">
+      <c r="AF13" s="9">
         <v>25</v>
       </c>
-      <c r="AG13" s="11">
+      <c r="AG13" s="9">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:33" s="1" customFormat="1" ht="41.65">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:33" s="1" customFormat="1">
+      <c r="A14" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="10">
         <v>6139</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I14" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14" s="12">
         <v>39878</v>
       </c>
-      <c r="L14" s="3">
+      <c r="L14" s="12">
         <v>39878</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="M14" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="N14" s="3">
+      <c r="N14" s="12">
         <v>39878</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="O14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="P14" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="Q14" s="1" t="s">
+      <c r="Q14" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="R14" s="1" t="s">
+      <c r="R14" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="S14" s="1" t="s">
+      <c r="S14" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="T14" s="1" t="s">
+      <c r="T14" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="U14" s="1" t="s">
+      <c r="U14" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="V14" s="1" t="s">
+      <c r="V14" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="W14" s="4" t="s">
+      <c r="W14" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="X14" s="1">
+      <c r="X14" s="10">
         <v>7.94</v>
       </c>
-      <c r="Y14" s="1">
+      <c r="Y14" s="10">
         <v>108</v>
       </c>
-      <c r="Z14" s="1">
+      <c r="Z14" s="10">
         <v>4050</v>
       </c>
-      <c r="AA14" s="4" t="s">
+      <c r="AA14" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="AB14" s="1" t="s">
+      <c r="AB14" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="AC14" s="1">
+      <c r="AC14" s="10">
         <v>37.5</v>
       </c>
-      <c r="AD14" s="1" t="s">
+      <c r="AD14" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="AE14" s="1">
+      <c r="AE14" s="10">
         <v>1.5</v>
       </c>
-      <c r="AF14" s="1">
+      <c r="AF14" s="10">
         <v>25</v>
       </c>
-      <c r="AG14" s="1" t="s">
+      <c r="AG14" s="10" t="s">
         <v>126</v>
       </c>
     </row>

</xml_diff>